<commit_message>
Finished The excel files will be edited in the computer of the user
</commit_message>
<xml_diff>
--- a/EmikoCoppermind/ExcelFiles/Abfuellraum_Handel.xlsx
+++ b/EmikoCoppermind/ExcelFiles/Abfuellraum_Handel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srv-ad\profiles$\f.camacho\Documents\ExcelFilesEmikoCoppermind\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.camacho\source\repos\EmikoCoppermind\EmikoCoppermind\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C73A69-1A28-484A-A0F9-BA0E9BB5A3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600E716A-AA55-4E00-B192-029433C3ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Some</t>
   </si>
@@ -36,13 +33,46 @@
     <t>data</t>
   </si>
   <si>
-    <t>Abfuellraum Handel</t>
-  </si>
-  <si>
     <t>This is abfuellraum</t>
   </si>
   <si>
     <t>handel file</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Patchfeld (von oben nach unten)</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Switch Anschluss (erste Zahl Switch, dann Port)</t>
+  </si>
+  <si>
+    <t>Büro</t>
+  </si>
+  <si>
+    <t>angeschl. Gerät/Computername</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>weitere Geräte</t>
+  </si>
+  <si>
+    <t>Weitere Ortsmerkmale</t>
+  </si>
+  <si>
+    <t>Besonderheiten</t>
+  </si>
+  <si>
+    <t>Blinkt nicht</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -59,7 +89,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -74,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,13 +112,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -369,39 +425,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>